<commit_message>
EPBDS-11682 added tests to test empty strings
</commit_message>
<xml_diff>
--- a/ITEST/itest.WebService/openl-repository/EPBDS-11682/EPBDS-11682/Main.xlsx
+++ b/ITEST/itest.WebService/openl-repository/EPBDS-11682/EPBDS-11682/Main.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\tomcats\apache-tomcat-8.5.35-openl\bin\openl-repository\Refactored HI Master Offer-DEFAULT-2021-06-18_17-27-12\Refactored HI Master Offer-DEFAULT-2021-06-18_17-27-12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EIS_Sources\OpenL\openl-tablets-clone\ITEST\itest.WebService\openl-repository\EPBDS-11682\EPBDS-11682\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7458B3-1DDB-4644-BF60-46948F179784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B1853F-DA62-4E26-B930-15DCFDFFCA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>= cond ? 1 : null</t>
   </si>
   <si>
-    <t>= cond ? "foo" : null</t>
-  </si>
-  <si>
     <t>Spreadsheet String StringResponse(Boolean cond)</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>Spreadsheet StringValue StringValueResponse(Boolean cond)</t>
+  </si>
+  <si>
+    <t>= cond == null ? "" : cond ? "foo" : null</t>
   </si>
 </sst>
 </file>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C10:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +455,7 @@
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.25">
@@ -476,7 +476,7 @@
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
@@ -518,7 +518,7 @@
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.25">
@@ -555,12 +555,12 @@
         <v>9</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>9</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>